<commit_message>
update readme + projet
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -857,7 +857,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="B11" s="4">
-        <f t="shared" ref="B11:B18" si="1">B10+1</f>
+        <f t="shared" ref="B11:B22" si="1">B10+1</f>
         <v>9</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -913,7 +913,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -955,7 +955,7 @@
     </row>
     <row r="19" ht="14.25">
       <c r="B19" s="4">
-        <f>B18+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C19" s="7"/>
@@ -965,7 +965,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="B20" s="4">
-        <f>B19+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C20" s="7"/>
@@ -975,7 +975,7 @@
     </row>
     <row r="21" ht="14.25">
       <c r="B21" s="4">
-        <f>B20+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C21" s="7"/>
@@ -985,7 +985,7 @@
     </row>
     <row r="22" ht="14.25">
       <c r="B22" s="4">
-        <f>B21+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="7"/>

</xml_diff>